<commit_message>
Tendría que estar estudiando física
</commit_message>
<xml_diff>
--- a/TP6/Mediciones.xlsx
+++ b/TP6/Mediciones.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\source\repos\TP3-Electro\TP6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70E55FD-4099-4055-9D34-0B7B369BA5C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA528757-44A2-4D9A-9BFA-503C3DA2C46D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="34">
   <si>
     <t>U_{RS}</t>
   </si>
@@ -151,7 +150,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,14 +159,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB8CCE4"/>
+        <fgColor rgb="FFD6E3BC"/>
+        <bgColor rgb="FFD6E3BC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor rgb="FFB8CCE4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD6E3BC"/>
-        <bgColor rgb="FFD6E3BC"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -242,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -253,38 +264,47 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -611,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -635,473 +655,342 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="5" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="11" t="s">
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="11" t="s">
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="11" t="s">
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="11" t="s">
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="11" t="s">
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="5" t="s">
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="W3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="X3" s="9" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26">
-      <c r="A3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="7">
-        <v>220</v>
-      </c>
-      <c r="E3" s="7">
-        <v>220</v>
-      </c>
-      <c r="F3" s="7">
-        <v>220</v>
-      </c>
-      <c r="G3" s="7">
-        <v>45</v>
-      </c>
-      <c r="H3" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="I3" s="7">
-        <f t="shared" ref="I3:I6" si="0">G3*H3</f>
-        <v>0.45</v>
-      </c>
-      <c r="J3" s="7">
-        <v>42</v>
-      </c>
-      <c r="K3" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="L3" s="7">
-        <f t="shared" ref="L3:L6" si="1">J3*K3</f>
-        <v>0.42</v>
-      </c>
-      <c r="M3" s="7">
-        <v>45</v>
-      </c>
-      <c r="N3" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="O3" s="7">
-        <f t="shared" ref="O3:O6" si="2">M3*N3</f>
-        <v>0.45</v>
-      </c>
-      <c r="P3" s="7">
-        <f t="shared" ref="P3:P6" si="3">R3/Q3</f>
-        <v>80</v>
-      </c>
-      <c r="Q3" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="R3" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="S3" s="7">
-        <f t="shared" ref="S3:S6" si="4">U3/T3</f>
-        <v>80</v>
-      </c>
-      <c r="T3" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="U3" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="V3" s="7">
-        <f t="shared" ref="V3:V6" si="5">X3/W3</f>
-        <v>80</v>
-      </c>
-      <c r="W3" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="X3" s="7">
-        <v>0.8</v>
       </c>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="6" t="s">
-        <v>18</v>
+      <c r="A4" s="5" t="s">
+        <v>17</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>18</v>
+      <c r="B4" s="5" t="s">
+        <v>17</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>18</v>
+      <c r="C4" s="5" t="s">
+        <v>17</v>
       </c>
-      <c r="D4" s="7">
-        <v>220</v>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6">
+        <f t="shared" ref="I4:I7" si="0">G4*H4</f>
+        <v>0</v>
       </c>
-      <c r="E4" s="7">
-        <v>220</v>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6">
+        <f t="shared" ref="L4:L7" si="1">J4*K4</f>
+        <v>0</v>
       </c>
-      <c r="F4" s="7">
-        <v>220</v>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6">
+        <f t="shared" ref="O4:O7" si="2">M4*N4</f>
+        <v>0</v>
       </c>
-      <c r="G4" s="7">
-        <v>83</v>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6">
+        <v>0.8</v>
       </c>
-      <c r="H4" s="7">
-        <v>0.01</v>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6">
+        <v>0.8</v>
       </c>
-      <c r="I4" s="7">
-        <f t="shared" si="0"/>
-        <v>0.83000000000000007</v>
-      </c>
-      <c r="J4" s="7">
-        <v>94</v>
-      </c>
-      <c r="K4" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="L4" s="7">
-        <f t="shared" si="1"/>
-        <v>0.94000000000000006</v>
-      </c>
-      <c r="M4" s="7">
-        <v>82</v>
-      </c>
-      <c r="N4" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="O4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.82000000000000006</v>
-      </c>
-      <c r="P4" s="7">
-        <f t="shared" si="3"/>
-        <v>28.999999999999996</v>
-      </c>
-      <c r="Q4" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="R4" s="7">
-        <v>1.45</v>
-      </c>
-      <c r="S4" s="7">
-        <f t="shared" si="4"/>
-        <v>32</v>
-      </c>
-      <c r="T4" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="U4" s="7">
-        <v>1.6</v>
-      </c>
-      <c r="V4" s="7">
-        <f t="shared" si="5"/>
-        <v>32.999999999999993</v>
-      </c>
-      <c r="W4" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="X4" s="7">
-        <v>1.65</v>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6">
+        <v>0.8</v>
       </c>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6">
+        <v>1.45</v>
+      </c>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="7">
-        <v>220</v>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
-      <c r="E5" s="7">
-        <v>220</v>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
-      <c r="F5" s="7">
-        <v>220</v>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
-      <c r="G5" s="7">
-        <v>92</v>
-      </c>
-      <c r="H5" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="I5" s="7">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-      <c r="J5" s="7">
-        <v>96</v>
-      </c>
-      <c r="K5" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="L5" s="7">
-        <f t="shared" si="1"/>
-        <v>0.96</v>
-      </c>
-      <c r="M5" s="7">
-        <v>90</v>
-      </c>
-      <c r="N5" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="O5" s="7">
-        <f t="shared" si="2"/>
-        <v>0.9</v>
-      </c>
-      <c r="P5" s="7">
-        <f t="shared" si="3"/>
-        <v>34</v>
-      </c>
-      <c r="Q5" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="R5" s="7">
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6">
         <v>1.7</v>
       </c>
-      <c r="S5" s="7">
-        <f t="shared" si="4"/>
-        <v>62</v>
-      </c>
-      <c r="T5" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="U5" s="7">
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6">
         <v>3.1</v>
       </c>
-      <c r="V5" s="7">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="W5" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="X5" s="7">
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
-      <c r="A6" s="6" t="s">
+    <row r="7" spans="1:26">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="7">
-        <v>220</v>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
-      <c r="E6" s="7">
-        <v>220</v>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
-      <c r="F6" s="7">
-        <v>220</v>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
-      <c r="G6" s="7">
-        <v>26</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="I6" s="7">
-        <f t="shared" si="0"/>
-        <v>0.26</v>
-      </c>
-      <c r="J6" s="7">
-        <v>94</v>
-      </c>
-      <c r="K6" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="L6" s="7">
-        <f t="shared" si="1"/>
-        <v>0.94000000000000006</v>
-      </c>
-      <c r="M6" s="7">
-        <v>80</v>
-      </c>
-      <c r="N6" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="O6" s="7">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
-      <c r="P6" s="7">
-        <f t="shared" si="3"/>
-        <v>13.999999999999998</v>
-      </c>
-      <c r="Q6" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="R6" s="7">
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6">
         <v>0.7</v>
       </c>
-      <c r="S6" s="7">
-        <f t="shared" si="4"/>
-        <v>52</v>
-      </c>
-      <c r="T6" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="U6" s="7">
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6">
         <v>2.6</v>
       </c>
-      <c r="V6" s="7">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="W6" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="X6" s="7">
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:26">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
@@ -1126,24 +1015,23 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
@@ -1152,89 +1040,89 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="5" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="11" t="s">
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="5" t="s">
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="9" t="s">
         <v>23</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="3"/>
+      <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="3"/>
+      <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="M11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" s="9" t="s">
         <v>25</v>
       </c>
       <c r="O11" s="1"/>
@@ -1249,50 +1137,36 @@
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="7">
-        <v>220</v>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6">
+        <f t="shared" ref="I12:I15" si="3">G12*H12</f>
+        <v>0</v>
       </c>
-      <c r="E12" s="7">
-        <v>220</v>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6">
+        <f t="shared" ref="L12:L15" si="4">J12*K12</f>
+        <v>0</v>
       </c>
-      <c r="F12" s="7">
-        <v>220</v>
+      <c r="M12" s="6">
+        <f t="shared" ref="M12:M15" si="5">I12+L12</f>
+        <v>0</v>
       </c>
-      <c r="G12" s="7">
-        <v>15</v>
-      </c>
-      <c r="H12" s="7">
-        <v>10</v>
-      </c>
-      <c r="I12" s="7">
-        <f t="shared" ref="I12:I15" si="6">G12*H12</f>
-        <v>150</v>
-      </c>
-      <c r="J12" s="7">
-        <v>15</v>
-      </c>
-      <c r="K12" s="7">
-        <v>10</v>
-      </c>
-      <c r="L12" s="7">
-        <f t="shared" ref="L12:L15" si="7">J12*K12</f>
-        <v>150</v>
-      </c>
-      <c r="M12" s="7">
-        <f t="shared" ref="M12:M15" si="8">I12+L12</f>
-        <v>300</v>
-      </c>
-      <c r="N12" s="7">
-        <f t="shared" ref="N12:N15" si="9">(I12-L12)*SQRT(3)</f>
+      <c r="N12" s="6">
+        <f t="shared" ref="N12:N15" si="6">(I12-L12)*SQRT(3)</f>
         <v>0</v>
       </c>
       <c r="O12" s="1"/>
@@ -1304,112 +1178,81 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
     </row>
     <row r="13" spans="1:26">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="7">
-        <v>220</v>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
-      <c r="E13" s="7">
-        <v>220</v>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
-      <c r="F13" s="7">
-        <v>220</v>
+      <c r="M13" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
-      <c r="G13" s="7">
-        <v>23</v>
-      </c>
-      <c r="H13" s="7">
-        <v>5</v>
-      </c>
-      <c r="I13" s="7">
+      <c r="N13" s="6">
         <f t="shared" si="6"/>
-        <v>115</v>
-      </c>
-      <c r="J13" s="7">
-        <v>4</v>
-      </c>
-      <c r="K13" s="7">
-        <v>5</v>
-      </c>
-      <c r="L13" s="7">
-        <f t="shared" si="7"/>
-        <v>20</v>
-      </c>
-      <c r="M13" s="7">
-        <f t="shared" si="8"/>
-        <v>135</v>
-      </c>
-      <c r="N13" s="7">
-        <f t="shared" si="9"/>
-        <v>164.54482671904333</v>
+        <v>0</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
+      <c r="R13" s="3"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
+      <c r="T13" s="3"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="7">
-        <v>220</v>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
-      <c r="E14" s="7">
-        <v>220</v>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
-      <c r="F14" s="7">
-        <v>220</v>
+      <c r="M14" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
-      <c r="G14" s="7">
-        <v>23</v>
-      </c>
-      <c r="H14" s="7">
-        <v>5</v>
-      </c>
-      <c r="I14" s="7">
+      <c r="N14" s="6">
         <f t="shared" si="6"/>
-        <v>115</v>
-      </c>
-      <c r="J14" s="7">
-        <v>11</v>
-      </c>
-      <c r="K14" s="7">
-        <v>5</v>
-      </c>
-      <c r="L14" s="7">
-        <f t="shared" si="7"/>
-        <v>55</v>
-      </c>
-      <c r="M14" s="7">
-        <f t="shared" si="8"/>
-        <v>170</v>
-      </c>
-      <c r="N14" s="7">
-        <f t="shared" si="9"/>
-        <v>103.92304845413263</v>
+        <v>0</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1419,55 +1262,39 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
     </row>
     <row r="15" spans="1:26">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="7">
-        <v>220</v>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
-      <c r="E15" s="7">
-        <v>220</v>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
-      <c r="F15" s="7">
-        <v>220</v>
+      <c r="M15" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
-      <c r="G15" s="7">
-        <v>4</v>
-      </c>
-      <c r="H15" s="7">
-        <v>5</v>
-      </c>
-      <c r="I15" s="7">
+      <c r="N15" s="6">
         <f t="shared" si="6"/>
-        <v>20</v>
-      </c>
-      <c r="J15" s="7">
-        <v>20</v>
-      </c>
-      <c r="K15" s="7">
-        <v>5</v>
-      </c>
-      <c r="L15" s="7">
-        <f t="shared" si="7"/>
-        <v>100</v>
-      </c>
-      <c r="M15" s="7">
-        <f t="shared" si="8"/>
-        <v>120</v>
-      </c>
-      <c r="N15" s="7">
-        <f t="shared" si="9"/>
-        <v>-138.56406460551017</v>
+        <v>0</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1477,8 +1304,6 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="1"/>
@@ -1503,10 +1328,8 @@
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-    </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1">
+    </row>
+    <row r="17" spans="1:25" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1515,10 +1338,12 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="I17" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1529,111 +1354,109 @@
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-    </row>
-    <row r="18" spans="1:26">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+    </row>
+    <row r="18" spans="1:25">
+      <c r="A18" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17">
+        <v>120</v>
+      </c>
+      <c r="E18" s="2"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="I18" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="17">
+        <v>30</v>
+      </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
-    </row>
-    <row r="19" spans="1:26">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+    </row>
+    <row r="19" spans="1:25">
+      <c r="A19" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="17">
+        <v>-120</v>
+      </c>
+      <c r="E19" s="2"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="I19" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="17">
+        <v>150</v>
+      </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="4"/>
-      <c r="Z19" s="4"/>
-    </row>
-    <row r="20" spans="1:26">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+    </row>
+    <row r="20" spans="1:25">
+      <c r="A20" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2"/>
       <c r="F20" s="1"/>
-      <c r="J20" s="3" t="s">
-        <v>26</v>
+      <c r="I20" s="16" t="s">
+        <v>29</v>
       </c>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="17">
+        <v>-90</v>
+      </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
-    </row>
-    <row r="21" spans="1:26">
-      <c r="A21" s="1"/>
-      <c r="B21" s="10" t="s">
-        <v>27</v>
+    </row>
+    <row r="21" spans="1:25">
+      <c r="A21" s="16" t="s">
+        <v>31</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="2">
-        <v>120</v>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17">
+        <f>0.7794</f>
+        <v>0.77939999999999998</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="E21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="10" t="s">
-        <v>27</v>
+      <c r="I21" s="16" t="s">
+        <v>31</v>
       </c>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="2">
-        <v>30</v>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="17">
+        <v>1.43</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1641,33 +1464,26 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-    </row>
-    <row r="22" spans="1:26">
-      <c r="A22" s="1"/>
-      <c r="B22" s="10" t="s">
-        <v>28</v>
+    </row>
+    <row r="22" spans="1:25">
+      <c r="A22" s="16" t="s">
+        <v>30</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="2">
-        <v>-120</v>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="18">
+        <v>0.71120000000000005</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="E22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="10" t="s">
-        <v>28</v>
+      <c r="I22" s="16" t="s">
+        <v>30</v>
       </c>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="2">
-        <v>150</v>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="17">
+        <v>1.53</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1678,30 +1494,25 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-    </row>
-    <row r="23" spans="1:26">
-      <c r="A23" s="1"/>
-      <c r="B23" s="10" t="s">
-        <v>29</v>
+    </row>
+    <row r="23" spans="1:25">
+      <c r="A23" s="16" t="s">
+        <v>32</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="2">
-        <v>0</v>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="19">
+        <v>7112</v>
       </c>
-      <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="10" t="s">
-        <v>29</v>
+      <c r="I23" s="16" t="s">
+        <v>33</v>
       </c>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="2">
-        <v>-90</v>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="17">
+        <v>1.53</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1712,17 +1523,16 @@
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-    </row>
-    <row r="24" spans="1:26">
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1738,17 +1548,16 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-    </row>
-    <row r="25" spans="1:26">
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+    </row>
+    <row r="25" spans="1:25">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1764,211 +1573,94 @@
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-    </row>
-    <row r="26" spans="1:26">
-      <c r="A26" s="1"/>
-      <c r="B26" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2">
-        <f>0.7794</f>
-        <v>0.77939999999999998</v>
-      </c>
+    </row>
+    <row r="26" spans="1:25">
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="8">
-        <v>1.4289000000000001</v>
-      </c>
+      <c r="M26" s="7"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="2">
-        <v>1.43</v>
-      </c>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
-    </row>
-    <row r="27" spans="1:26">
+    </row>
+    <row r="27" spans="1:25">
       <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-    </row>
-    <row r="28" spans="1:26">
+    </row>
+    <row r="28" spans="1:25">
       <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
+      <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
-    </row>
-    <row r="29" spans="1:26">
-      <c r="A29" s="1"/>
-      <c r="B29" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="8">
-        <v>0.71120000000000005</v>
-      </c>
+    </row>
+    <row r="29" spans="1:25">
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="8"/>
+      <c r="M29" s="7"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="2">
-        <v>1.53</v>
-      </c>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
-    </row>
-    <row r="30" spans="1:26">
+    </row>
+    <row r="30" spans="1:25">
       <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
-      <c r="X30" s="1"/>
-    </row>
-    <row r="31" spans="1:26">
+    </row>
+    <row r="31" spans="1:25">
       <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
-    </row>
-    <row r="32" spans="1:26">
+    </row>
+    <row r="32" spans="1:25">
       <c r="A32" s="1"/>
-      <c r="B32" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="9">
-        <v>7112</v>
-      </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
-      <c r="I32" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
-      <c r="O32" s="2">
-        <v>1.53</v>
-      </c>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
-      <c r="W32" s="1"/>
-      <c r="X32" s="1"/>
     </row>
     <row r="33" spans="1:24">
       <c r="C33" s="2"/>
@@ -27099,475 +26791,38 @@
       <c r="X1000" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="V1:X1"/>
+  <mergeCells count="25">
+    <mergeCell ref="A1:X1"/>
+    <mergeCell ref="A9:N9"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="V2:X2"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="J10:L10"/>
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="S2:U2"/>
   </mergeCells>
-  <conditionalFormatting sqref="F29 M29">
+  <conditionalFormatting sqref="D22 M29">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(F29))&gt;0</formula>
+      <formula>LEN(TRIM(D22))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="26" width="10.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-    </row>
-    <row r="2" spans="1:24">
-      <c r="A2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="V2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="X2" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="7">
-        <v>102</v>
-      </c>
-      <c r="E3" s="7">
-        <v>104</v>
-      </c>
-      <c r="F3" s="7">
-        <v>101</v>
-      </c>
-      <c r="G3" s="7">
-        <v>150</v>
-      </c>
-      <c r="H3" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="I3" s="7">
-        <v>0.89</v>
-      </c>
-      <c r="J3" s="7">
-        <v>150</v>
-      </c>
-      <c r="K3" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="L3" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="M3" s="7">
-        <v>150</v>
-      </c>
-      <c r="N3" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="O3" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="P3" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="7">
-        <v>1</v>
-      </c>
-      <c r="R3" s="7">
-        <v>1.55</v>
-      </c>
-      <c r="S3" s="7">
-        <v>2</v>
-      </c>
-      <c r="T3" s="7">
-        <v>1</v>
-      </c>
-      <c r="U3" s="7">
-        <v>1.56</v>
-      </c>
-      <c r="V3" s="7">
-        <v>2</v>
-      </c>
-      <c r="W3" s="7">
-        <v>1</v>
-      </c>
-      <c r="X3" s="7">
-        <v>1.58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
-      <c r="A4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="7">
-        <v>102</v>
-      </c>
-      <c r="E4" s="7">
-        <v>104</v>
-      </c>
-      <c r="F4" s="7">
-        <v>102</v>
-      </c>
-      <c r="G4" s="7">
-        <v>150</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="I4" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="J4" s="7">
-        <v>150</v>
-      </c>
-      <c r="K4" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="L4" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="M4" s="7">
-        <v>150</v>
-      </c>
-      <c r="N4" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="O4" s="7">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="P4" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="7">
-        <v>1</v>
-      </c>
-      <c r="R4" s="7">
-        <v>1.8</v>
-      </c>
-      <c r="S4" s="7">
-        <v>2</v>
-      </c>
-      <c r="T4" s="7">
-        <v>1</v>
-      </c>
-      <c r="U4" s="7">
-        <v>1.61</v>
-      </c>
-      <c r="V4" s="7">
-        <v>2</v>
-      </c>
-      <c r="W4" s="7">
-        <v>1</v>
-      </c>
-      <c r="X4" s="7">
-        <v>1.84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24">
-      <c r="A5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="7">
-        <v>99</v>
-      </c>
-      <c r="E5" s="7">
-        <v>100</v>
-      </c>
-      <c r="F5" s="7">
-        <v>98</v>
-      </c>
-      <c r="G5" s="7">
-        <v>300</v>
-      </c>
-      <c r="H5" s="7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="I5" s="7">
-        <v>1.35</v>
-      </c>
-      <c r="J5" s="7">
-        <v>300</v>
-      </c>
-      <c r="K5" s="7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="L5" s="7">
-        <v>1.425</v>
-      </c>
-      <c r="M5" s="7">
-        <v>300</v>
-      </c>
-      <c r="N5" s="7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="O5" s="7">
-        <v>1.6</v>
-      </c>
-      <c r="P5" s="7">
-        <v>5</v>
-      </c>
-      <c r="Q5" s="7">
-        <v>1</v>
-      </c>
-      <c r="R5" s="7">
-        <v>2.5</v>
-      </c>
-      <c r="S5" s="7">
-        <v>5</v>
-      </c>
-      <c r="T5" s="7">
-        <v>1</v>
-      </c>
-      <c r="U5" s="7">
-        <v>2.4</v>
-      </c>
-      <c r="V5" s="7">
-        <v>5</v>
-      </c>
-      <c r="W5" s="7">
-        <v>1</v>
-      </c>
-      <c r="X5" s="7">
-        <v>2.65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
-      <c r="A6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="7">
-        <v>102</v>
-      </c>
-      <c r="E6" s="7">
-        <v>101</v>
-      </c>
-      <c r="F6" s="7">
-        <v>101.5</v>
-      </c>
-      <c r="G6" s="7">
-        <v>150</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="I6" s="7">
-        <v>0.89</v>
-      </c>
-      <c r="J6" s="7">
-        <v>150</v>
-      </c>
-      <c r="K6" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="L6" s="7">
-        <v>1.39</v>
-      </c>
-      <c r="M6" s="7">
-        <v>150</v>
-      </c>
-      <c r="N6" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="O6" s="7">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="P6" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="7">
-        <v>1</v>
-      </c>
-      <c r="R6" s="7">
-        <v>0.84</v>
-      </c>
-      <c r="S6" s="7">
-        <v>5</v>
-      </c>
-      <c r="T6" s="7">
-        <v>1</v>
-      </c>
-      <c r="U6" s="7">
-        <v>2.25</v>
-      </c>
-      <c r="V6" s="7">
-        <v>5</v>
-      </c>
-      <c r="W6" s="7">
-        <v>1</v>
-      </c>
-      <c r="X6" s="7">
-        <v>2.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="S1:U1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Hacer diagramas fasoriales con la tercer tabla
</commit_message>
<xml_diff>
--- a/TP6/Mediciones.xlsx
+++ b/TP6/Mediciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellon\source\repos\TPs-Electro\TP6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C52206-5EFB-417E-B7F7-066AD0CD3BDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A976022-CBD9-4CE4-A943-88278FDB62F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="43">
   <si>
     <t>U_{RS}</t>
   </si>
@@ -157,15 +157,6 @@
     <t>En grados</t>
   </si>
   <si>
-    <t>$I_{R}$ = $I_{RS}$ - $I_{TR}$</t>
-  </si>
-  <si>
-    <t>$I_{S}$ = $I_{ST}$ - $I_{RS}$</t>
-  </si>
-  <si>
-    <t>$I_{T}$ = $I_{TR}$ - $I_{ST}$</t>
-  </si>
-  <si>
     <t>Modulo</t>
   </si>
 </sst>
@@ -175,7 +166,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -233,7 +224,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -252,32 +243,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -320,33 +285,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -375,41 +318,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -425,27 +340,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:F20"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -786,7 +712,7 @@
     <col min="8" max="8" width="7.42578125" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" customWidth="1"/>
     <col min="12" max="12" width="9.5703125" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" customWidth="1"/>
     <col min="14" max="14" width="7.42578125" customWidth="1"/>
@@ -801,39 +727,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
       <c r="D2" s="8" t="s">
         <v>0</v>
       </c>
@@ -843,36 +769,36 @@
       <c r="F2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="13" t="s">
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="13" t="s">
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="13" t="s">
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="13" t="s">
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="13" t="s">
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="11" t="s">
@@ -1298,22 +1224,22 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
@@ -1326,11 +1252,11 @@
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="8" t="s">
         <v>0</v>
       </c>
@@ -1340,16 +1266,16 @@
       <c r="F10" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="13" t="s">
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
       <c r="M10" s="8" t="s">
         <v>19</v>
       </c>
@@ -1678,11 +1604,11 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -1694,32 +1620,38 @@
       <c r="V17" s="4"/>
     </row>
     <row r="18" spans="1:25">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="33" t="s">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
+      <c r="E18" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18" s="21"/>
+      <c r="M18" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="N18" s="17"/>
+      <c r="O18" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="P18" s="21"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="4"/>
     </row>
@@ -1736,30 +1668,42 @@
       <c r="D19" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="36"/>
-      <c r="G19" s="33" t="s">
+      <c r="E19" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H19" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="I19" s="36"/>
-      <c r="J19" s="33" t="s">
+      <c r="G19" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="K19" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="L19" s="36"/>
-      <c r="M19" s="33" t="s">
+      <c r="I19" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="N19" s="30"/>
-      <c r="O19" s="30"/>
-      <c r="P19" s="30"/>
+      <c r="K19" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M19" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="N19" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="O19" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="P19" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
@@ -1773,22 +1717,55 @@
       <c r="C20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20" s="14">
         <f>ATAN(SQRT(3)*(I12-L12)/(I12+L12))*180/PI()</f>
         <v>1.245484135405325</v>
       </c>
-      <c r="E20" s="34"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
+      <c r="E20" s="6">
+        <f>D4</f>
+        <v>140</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0</v>
+      </c>
+      <c r="G20" s="6">
+        <f>E4</f>
+        <v>137.19999999999999</v>
+      </c>
+      <c r="H20" s="6">
+        <v>120</v>
+      </c>
+      <c r="I20" s="6">
+        <f>F4</f>
+        <v>137.5</v>
+      </c>
+      <c r="J20" s="6">
+        <v>-120</v>
+      </c>
+      <c r="K20" s="6">
+        <f>R4</f>
+        <v>2.0750000000000002</v>
+      </c>
+      <c r="L20" s="6">
+        <f>F20/D20</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="6">
+        <f>U4</f>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="N20" s="30">
+        <f>H20/D20</f>
+        <v>96.348075891747683</v>
+      </c>
+      <c r="O20" s="6">
+        <f>X4</f>
+        <v>3.7</v>
+      </c>
+      <c r="P20" s="30">
+        <f>J20/D20</f>
+        <v>-96.348075891747683</v>
+      </c>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
@@ -1802,19 +1779,55 @@
       <c r="C21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="14">
         <f t="shared" ref="D21:D23" si="10">ATAN(SQRT(3)*(I13-L13)/(I13+L13))*180/PI()</f>
         <v>29.324934632214219</v>
       </c>
-      <c r="E21" s="34"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="9"/>
+      <c r="E21" s="6">
+        <f t="shared" ref="E21:E23" si="11">D5</f>
+        <v>140</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
+        <f t="shared" ref="G21:G23" si="12">E5</f>
+        <v>137.19999999999999</v>
+      </c>
+      <c r="H21" s="6">
+        <v>120</v>
+      </c>
+      <c r="I21" s="6">
+        <f t="shared" ref="I21:I23" si="13">F5</f>
+        <v>137.5</v>
+      </c>
+      <c r="J21" s="6">
+        <v>-120</v>
+      </c>
+      <c r="K21" s="6">
+        <f t="shared" ref="K21:K23" si="14">R5</f>
+        <v>1.55</v>
+      </c>
+      <c r="L21" s="6">
+        <f t="shared" ref="L21:L23" si="15">F21/D21</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="6">
+        <f t="shared" ref="M21:M23" si="16">U5</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N21" s="30">
+        <f t="shared" ref="N21:N23" si="17">H21/D21</f>
+        <v>4.0920807328305795</v>
+      </c>
+      <c r="O21" s="6">
+        <f t="shared" ref="O21:O23" si="18">X5</f>
+        <v>2.9</v>
+      </c>
+      <c r="P21" s="30">
+        <f t="shared" ref="P21:P23" si="19">J21/D21</f>
+        <v>-4.0920807328305795</v>
+      </c>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
@@ -1828,19 +1841,55 @@
       <c r="C22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="14">
         <f t="shared" si="10"/>
         <v>40.893394649130911</v>
       </c>
-      <c r="E22" s="34"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="22"/>
+      <c r="E22" s="6">
+        <f t="shared" si="11"/>
+        <v>140</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0</v>
+      </c>
+      <c r="G22" s="6">
+        <f t="shared" si="12"/>
+        <v>137.19999999999999</v>
+      </c>
+      <c r="H22" s="6">
+        <v>120</v>
+      </c>
+      <c r="I22" s="6">
+        <f t="shared" si="13"/>
+        <v>137.5</v>
+      </c>
+      <c r="J22" s="6">
+        <v>-120</v>
+      </c>
+      <c r="K22" s="6">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="L22" s="6">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="6">
+        <f t="shared" si="16"/>
+        <v>3.4</v>
+      </c>
+      <c r="N22" s="30">
+        <f t="shared" si="17"/>
+        <v>2.9344592453038207</v>
+      </c>
+      <c r="O22" s="6">
+        <f t="shared" si="18"/>
+        <v>4.5</v>
+      </c>
+      <c r="P22" s="30">
+        <f t="shared" si="19"/>
+        <v>-2.9344592453038207</v>
+      </c>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
     </row>
@@ -1854,19 +1903,55 @@
       <c r="C23" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="14">
         <f t="shared" si="10"/>
         <v>-32.13319017374581</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="9"/>
+      <c r="E23" s="6">
+        <f t="shared" si="11"/>
+        <v>140</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0</v>
+      </c>
+      <c r="G23" s="6">
+        <f t="shared" si="12"/>
+        <v>137.19999999999999</v>
+      </c>
+      <c r="H23" s="6">
+        <v>120</v>
+      </c>
+      <c r="I23" s="6">
+        <f t="shared" si="13"/>
+        <v>137.5</v>
+      </c>
+      <c r="J23" s="6">
+        <v>-120</v>
+      </c>
+      <c r="K23" s="6">
+        <f t="shared" si="14"/>
+        <v>1.05</v>
+      </c>
+      <c r="L23" s="6">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="6">
+        <f t="shared" si="16"/>
+        <v>2.95</v>
+      </c>
+      <c r="N23" s="30">
+        <f t="shared" si="17"/>
+        <v>-3.7344564716778459</v>
+      </c>
+      <c r="O23" s="6">
+        <f t="shared" si="18"/>
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="P23" s="30">
+        <f t="shared" si="19"/>
+        <v>3.7344564716778459</v>
+      </c>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
@@ -1882,13 +1967,15 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
       <c r="P24" s="1"/>
@@ -1907,7 +1994,9 @@
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1924,7 +2013,9 @@
       <c r="U25" s="1"/>
     </row>
     <row r="26" spans="1:25">
-      <c r="G26" s="2"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
       <c r="H26" s="2"/>
       <c r="M26" s="7"/>
       <c r="N26" s="2"/>
@@ -1939,7 +2030,9 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
       <c r="H27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -1954,7 +2047,9 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
       <c r="H28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -1965,7 +2060,9 @@
       <c r="U28" s="1"/>
     </row>
     <row r="29" spans="1:25">
-      <c r="G29" s="2"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
       <c r="H29" s="2"/>
       <c r="M29" s="7"/>
       <c r="N29" s="2"/>
@@ -1977,7 +2074,9 @@
     </row>
     <row r="30" spans="1:25">
       <c r="A30" s="1"/>
-      <c r="G30" s="2"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
       <c r="H30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -27140,26 +27239,7 @@
       <c r="X1000" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
+  <mergeCells count="18">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="G2:I2"/>
@@ -27172,6 +27252,12 @@
     <mergeCell ref="S2:U2"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="J10:L10"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A18:C18"/>
   </mergeCells>
   <conditionalFormatting sqref="M29">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -27194,52 +27280,52 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="21"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="28"/>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="26" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="L2" s="16" t="s">
         <v>35</v>
       </c>
     </row>
@@ -27253,31 +27339,31 @@
       <c r="C3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="13" t="s">
         <v>24</v>
       </c>
     </row>
@@ -27458,22 +27544,22 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="11" t="s">
         <v>25</v>
       </c>
@@ -27534,7 +27620,7 @@
         <f>Hoja1!$M12</f>
         <v>478</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="15">
         <f>Hoja1!$N12</f>
         <v>10.392304845413264</v>
       </c>
@@ -27561,7 +27647,7 @@
         <f>Hoja1!$M13</f>
         <v>296</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="15">
         <f>Hoja1!$N13</f>
         <v>166.27687752661222</v>
       </c>
@@ -27588,7 +27674,7 @@
         <f>Hoja1!$M14</f>
         <v>528</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="15">
         <f>Hoja1!$N14</f>
         <v>457.26141319818356</v>
       </c>
@@ -27615,7 +27701,7 @@
         <f>Hoja1!$M15</f>
         <v>364</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="15">
         <f>Hoja1!$N15</f>
         <v>-228.63070659909178</v>
       </c>

</xml_diff>